<commit_message>
uniones paneles casi todas (cierre)
</commit_message>
<xml_diff>
--- a/GUI/FuncionEstimacionMAsa.xlsx
+++ b/GUI/FuncionEstimacionMAsa.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/anaisabel_soria_alumnos_upm_es/Documents/Escritorio/UPM/IGA/PBL/Satellite-Module-Design-PBL/GUI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{C8415831-075E-4181-8B1E-353C9B4EB6C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9430496F-582A-4B42-A9AD-DEEC0E17794B}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{C8415831-075E-4181-8B1E-353C9B4EB6C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{49C6BFE8-94E6-40B8-B71B-77B16681A1E4}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="340" windowWidth="24290" windowHeight="15860" xr2:uid="{212450EA-A04A-47F1-9981-3B068E7A7DBE}"/>
+    <workbookView xWindow="340" yWindow="340" windowWidth="24290" windowHeight="15860" activeTab="1" xr2:uid="{212450EA-A04A-47F1-9981-3B068E7A7DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Al6061" sheetId="1" r:id="rId1"/>
+    <sheet name="CFRP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>LADO</t>
   </si>
@@ -84,8 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,6 +953,844 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Geometría hexagonal</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17002531290958384"/>
+          <c:y val="3.7037037037037035E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.10106977252843395"/>
+                  <c:y val="-0.19492855059784195"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CFRP!$F$5:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CFRP!$G$5:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.4119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2410000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9129999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.452</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3109999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4EC4-4EB1-9AA7-60B9A31A0703}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1230576672"/>
+        <c:axId val="1230572096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1230576672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1230572096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1230572096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1230576672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Geometria cuadrada</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22971522309711287"/>
+          <c:y val="1.8518518518518517E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.12905883639545057"/>
+                  <c:y val="-0.18549394867308253"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CFRP!$A$6:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CFRP!$B$6:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5910000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3479999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1109999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8809999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6579999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9895-4B0B-A84C-6748BFEE117C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1223288192"/>
+        <c:axId val="1223306912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1223288192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1223306912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1223306912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1223288192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1029,6 +1871,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1546,6 +2468,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2118,6 +4072,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{930DE695-D946-4B0F-8EFB-28BD7588CF5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0A6A69C-8F11-4833-BBA8-C4528F8CF1F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC4C743-8D97-4C98-BCC9-F4B6027F8DC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2437,21 +4468,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936F92E9-409F-462C-B1A0-8CEDEA08E67E}">
   <dimension ref="A5:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="K5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="K5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -2616,4 +4647,186 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338FB669-8F01-483E-A0D9-F2346EDF0654}">
+  <dimension ref="A3:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>400</v>
+      </c>
+      <c r="G5">
+        <v>3.4119999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>400</v>
+      </c>
+      <c r="B6">
+        <v>5.0960000000000001</v>
+      </c>
+      <c r="F6">
+        <v>390</v>
+      </c>
+      <c r="G6">
+        <v>3.2410000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>390</v>
+      </c>
+      <c r="B7">
+        <v>4.84</v>
+      </c>
+      <c r="F7">
+        <v>380</v>
+      </c>
+      <c r="G7">
+        <v>3.0750000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>380</v>
+      </c>
+      <c r="B8">
+        <v>4.5910000000000002</v>
+      </c>
+      <c r="F8">
+        <v>370</v>
+      </c>
+      <c r="G8">
+        <v>2.9129999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>370</v>
+      </c>
+      <c r="B9">
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="F9">
+        <v>360</v>
+      </c>
+      <c r="G9">
+        <v>2.7549999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>360</v>
+      </c>
+      <c r="B10">
+        <v>4.1109999999999998</v>
+      </c>
+      <c r="F10">
+        <v>350</v>
+      </c>
+      <c r="G10">
+        <v>2.6019999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>350</v>
+      </c>
+      <c r="B11">
+        <v>3.8809999999999998</v>
+      </c>
+      <c r="F11">
+        <v>340</v>
+      </c>
+      <c r="G11">
+        <v>2.452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>340</v>
+      </c>
+      <c r="B12">
+        <v>3.6579999999999999</v>
+      </c>
+      <c r="F12">
+        <v>330</v>
+      </c>
+      <c r="G12">
+        <v>2.3109999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>330</v>
+      </c>
+      <c r="B13">
+        <v>3.44</v>
+      </c>
+      <c r="F13">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>320</v>
+      </c>
+      <c r="F14">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>300</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>